<commit_message>
added new resources to OR and DataEngine
Git test 1
</commit_message>
<xml_diff>
--- a/Bumrise/src/dataEngine/DataEngine.xlsx
+++ b/Bumrise/src/dataEngine/DataEngine.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Bumrise\src\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BumGit\bum-repository\Bumrise\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -145,9 +145,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Login_02</t>
-  </si>
-  <si>
     <t>TS_009</t>
   </si>
   <si>
@@ -233,13 +230,36 @@
   </si>
   <si>
     <t>Inventory_Page Objects</t>
+  </si>
+  <si>
+    <t>Action_01</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>TS_012</t>
+  </si>
+  <si>
+    <t>TS_013</t>
+  </si>
+  <si>
+    <t>TS_014</t>
+  </si>
+  <si>
+    <t>TS_015</t>
+  </si>
+  <si>
+    <t>Click Action</t>
+  </si>
+  <si>
+    <t>Collect Bottles for 1 Hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -334,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -356,6 +376,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,19 +660,19 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -665,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>26</v>
@@ -674,10 +695,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -697,7 +718,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,7 +738,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,7 +758,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -745,25 +766,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -777,19 +798,19 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -813,7 +834,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -833,7 +854,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,16 +865,16 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -861,13 +882,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>30</v>
@@ -877,7 +898,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -885,7 +906,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -897,53 +918,81 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="A12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1064,13 +1113,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D16">
       <formula1>Page_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F16">
       <formula1>Action_Keywords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E16">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1084,14 +1133,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1105,7 +1154,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1119,15 +1168,15 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>35</v>
@@ -1145,46 +1194,46 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G24"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="E1" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
@@ -1193,13 +1242,13 @@
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
@@ -1207,18 +1256,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
@@ -1226,13 +1275,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1243,7 +1292,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1251,12 +1300,12 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1264,7 +1313,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,7 +1346,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added Empty test step
</commit_message>
<xml_diff>
--- a/Bumrise/src/dataEngine/DataEngine.xlsx
+++ b/Bumrise/src/dataEngine/DataEngine.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BumGit\bum-repository\Bumrise\src\dataEngine\"/>
     </mc:Choice>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -326,12 +326,52 @@
   </si>
   <si>
     <t>TS_025</t>
+  </si>
+  <si>
+    <t>Empty_01</t>
+  </si>
+  <si>
+    <t>TS_026</t>
+  </si>
+  <si>
+    <t>TS_027</t>
+  </si>
+  <si>
+    <t>TS_028</t>
+  </si>
+  <si>
+    <t>TS_029</t>
+  </si>
+  <si>
+    <t>TS_030</t>
+  </si>
+  <si>
+    <t>Go to homepage</t>
+  </si>
+  <si>
+    <t>TS_031</t>
+  </si>
+  <si>
+    <t>btn_Home</t>
+  </si>
+  <si>
+    <t>Close pop-up</t>
+  </si>
+  <si>
+    <t>Click Empty</t>
+  </si>
+  <si>
+    <t>Empty collected bottles</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -732,19 +772,19 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,27 +1287,24 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -1277,68 +1314,153 @@
         <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1" t="s">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="1"/>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="A30" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="A31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="A32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -1405,13 +1527,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D32">
       <formula1>Page_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31">
       <formula1>Action_Keywords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1422,17 +1544,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1482,21 +1604,38 @@
         <v>71</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>91</v>
+      <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1510,18 +1649,18 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1752,9 @@
         <v>50</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>

</xml_diff>

<commit_message>
modified the Collect button xpath
</commit_message>
<xml_diff>
--- a/Bumrise/src/dataEngine/DataEngine.xlsx
+++ b/Bumrise/src/dataEngine/DataEngine.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BumGit\bum-repository\Bumrise\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="6270" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="6270"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="110">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -371,7 +371,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -771,20 +770,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1219,6 +1218,9 @@
         <v>18</v>
       </c>
       <c r="G21" s="1"/>
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1236,6 +1238,9 @@
         <v>38</v>
       </c>
       <c r="G22" s="1"/>
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -1305,6 +1310,9 @@
         <v>31</v>
       </c>
       <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -1327,7 +1335,7 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,7 +1379,7 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1435,7 +1443,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1547,14 +1555,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -1604,7 +1612,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>93</v>
@@ -1618,10 +1626,10 @@
         <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,19 +1656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>